<commit_message>
add caption and edit some text
</commit_message>
<xml_diff>
--- a/draft/chapter1.xlsx
+++ b/draft/chapter1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinki\Desktop\publish\draft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinki.lee\publish\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>&lt;unk&gt;</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>i'm,&lt;unk&gt;:</t>
+  </si>
+  <si>
+    <t>표1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -464,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T30"/>
+  <dimension ref="B3:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5:X35"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -508,6 +520,9 @@
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="1">
         <v>10</v>
       </c>
@@ -947,7 +962,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
@@ -988,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S18" t="s">
         <v>19</v>
       </c>
@@ -996,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S19" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>0</v>
@@ -1043,7 +1061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1292,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1337,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1382,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1427,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
@@ -1472,7 +1490,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>